<commit_message>
Sorting rooms in number order
</commit_message>
<xml_diff>
--- a/ENGR1020/rooms.xlsx
+++ b/ENGR1020/rooms.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\conno.CONNORMINI\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9723816-87E3-4445-99CF-35C0DDE97787}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{757E490D-D505-4B68-AE7C-9F2BA3ABB990}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{5FB6F6AD-C0A2-D447-82DA-0B46727E9FA3}"/>
   </bookViews>
@@ -682,8 +682,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A88781D-DB75-8C49-AAFE-30EFB83A7475}">
   <dimension ref="A1:C92"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="101" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="101" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
@@ -705,216 +705,216 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A2">
-        <v>1073</v>
+        <v>1025</v>
       </c>
       <c r="B2" t="s">
-        <v>0</v>
+        <v>82</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A3">
-        <v>1025</v>
+        <v>1027</v>
       </c>
       <c r="B3" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A4">
-        <v>1027</v>
+        <v>1041</v>
       </c>
       <c r="B4" t="s">
-        <v>83</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A5">
-        <v>1041</v>
+        <v>1042</v>
       </c>
       <c r="B5" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A6">
-        <v>1042</v>
+        <v>1073</v>
       </c>
       <c r="B6" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A7">
-        <v>1205</v>
+        <v>1111</v>
       </c>
       <c r="B7" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A8">
-        <v>1207</v>
+        <v>1113</v>
       </c>
       <c r="B8" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A9">
-        <v>1213</v>
+        <v>1115</v>
       </c>
       <c r="B9" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" t="s">
-        <v>78</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A10">
-        <v>1111</v>
+        <v>1117</v>
       </c>
       <c r="B10" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A11">
-        <v>1113</v>
+        <v>1119</v>
       </c>
       <c r="B11" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A12">
-        <v>1215</v>
+        <v>1121</v>
       </c>
       <c r="B12" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A13">
-        <v>1217</v>
+        <v>1123</v>
       </c>
       <c r="B13" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A14">
-        <v>1115</v>
+        <v>1125</v>
       </c>
       <c r="B14" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A15">
-        <v>1117</v>
+        <v>1127</v>
       </c>
       <c r="B15" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A16">
+        <v>1129</v>
+      </c>
+      <c r="B16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A17">
+        <v>1131</v>
+      </c>
+      <c r="B17" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A18">
+        <v>1133</v>
+      </c>
+      <c r="B18" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A19">
+        <v>1205</v>
+      </c>
+      <c r="B19" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A20">
+        <v>1207</v>
+      </c>
+      <c r="B20" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A21">
+        <v>1213</v>
+      </c>
+      <c r="B21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C21" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A22">
+        <v>1215</v>
+      </c>
+      <c r="B22" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A23">
+        <v>1217</v>
+      </c>
+      <c r="B23" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A24">
         <v>1219</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B24" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A17">
-        <v>1119</v>
-      </c>
-      <c r="B17" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A18">
-        <v>1121</v>
-      </c>
-      <c r="B18" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A19">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A25">
         <v>1225</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B25" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A20">
-        <v>1123</v>
-      </c>
-      <c r="B20" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A21">
-        <v>1125</v>
-      </c>
-      <c r="B21" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A22">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A26">
         <v>1227</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B26" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A23">
-        <v>1127</v>
-      </c>
-      <c r="B23" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A24">
-        <v>1129</v>
-      </c>
-      <c r="B24" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A27">
         <v>1231</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B27" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A26">
-        <v>1131</v>
-      </c>
-      <c r="B26" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A27">
-        <v>1133</v>
-      </c>
-      <c r="B27" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A28">
         <v>1237</v>
       </c>
@@ -922,23 +922,23 @@
         <v>22</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A29">
+        <v>1261</v>
+      </c>
+      <c r="B29" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A30">
         <v>1262</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B30" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A30">
-        <v>1261</v>
-      </c>
-      <c r="B30" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A31">
         <v>2001</v>
       </c>
@@ -946,506 +946,508 @@
         <v>23</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A32">
-        <v>2073</v>
+        <v>2010</v>
       </c>
       <c r="B32" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A33">
-        <v>2010</v>
+        <v>2013</v>
       </c>
       <c r="B33" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A34">
-        <v>2013</v>
+        <v>2014</v>
       </c>
       <c r="B34" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A35">
-        <v>2014</v>
+        <v>2019</v>
       </c>
       <c r="B35" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A36">
-        <v>2019</v>
+        <v>2025</v>
       </c>
       <c r="B36" t="s">
-        <v>28</v>
+        <v>86</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A37">
-        <v>2025</v>
+        <v>2027</v>
       </c>
       <c r="B37" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A38">
-        <v>2027</v>
+        <v>2041</v>
       </c>
       <c r="B38" t="s">
-        <v>87</v>
+        <v>29</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A39">
-        <v>2041</v>
+      <c r="A39" s="1">
+        <v>2042</v>
       </c>
       <c r="B39" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A40" s="1" t="s">
-        <v>30</v>
+      <c r="A40" s="1">
+        <v>2051</v>
       </c>
       <c r="B40" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A41" s="1">
-        <v>2051</v>
+      <c r="A41">
+        <v>2073</v>
       </c>
       <c r="B41" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A42" s="1" t="s">
-        <v>33</v>
+      <c r="A42" s="1">
+        <v>2111</v>
       </c>
       <c r="B42" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A43" s="1">
-        <v>2042</v>
+        <v>2113</v>
       </c>
       <c r="B43" t="s">
-        <v>35</v>
+        <v>61</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A44" s="1">
-        <v>2204</v>
+        <v>2115</v>
       </c>
       <c r="B44" t="s">
-        <v>3</v>
+        <v>63</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A45" s="1">
-        <v>2206</v>
+        <v>2117</v>
       </c>
       <c r="B45" t="s">
-        <v>3</v>
+        <v>64</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A46" s="1">
-        <v>2304</v>
+        <v>2119</v>
       </c>
       <c r="B46" t="s">
-        <v>3</v>
+        <v>66</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A47" s="1">
-        <v>2302</v>
+        <v>2121</v>
       </c>
       <c r="B47" t="s">
-        <v>3</v>
+        <v>67</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A48" s="1">
-        <v>2208</v>
+        <v>2123</v>
       </c>
       <c r="B48" t="s">
-        <v>36</v>
+        <v>69</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A49" s="1">
-        <v>2214</v>
+        <v>2125</v>
       </c>
       <c r="B49" t="s">
-        <v>37</v>
+        <v>70</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A50" s="1">
-        <v>2312</v>
+        <v>2127</v>
       </c>
       <c r="B50" t="s">
-        <v>38</v>
+        <v>72</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A51" s="1">
-        <v>2314</v>
+        <v>2129</v>
       </c>
       <c r="B51" t="s">
-        <v>39</v>
+        <v>73</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A52" s="1">
-        <v>2216</v>
+        <v>2131</v>
       </c>
       <c r="B52" t="s">
-        <v>40</v>
+        <v>75</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A53" s="1">
-        <v>2316</v>
+        <v>2133</v>
       </c>
       <c r="B53" t="s">
-        <v>41</v>
+        <v>76</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A54" s="1">
-        <v>2318</v>
+        <v>2201</v>
       </c>
       <c r="B54" t="s">
-        <v>42</v>
+        <v>56</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A55" s="1">
-        <v>2220</v>
+        <v>2203</v>
       </c>
       <c r="B55" t="s">
-        <v>43</v>
+        <v>3</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A56" s="1">
-        <v>2320</v>
+        <v>2204</v>
       </c>
       <c r="B56" t="s">
-        <v>44</v>
+        <v>3</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A57" s="1">
-        <v>2322</v>
+        <v>2205</v>
       </c>
       <c r="B57" t="s">
-        <v>45</v>
+        <v>57</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A58" s="1">
-        <v>2226</v>
+        <v>2206</v>
       </c>
       <c r="B58" t="s">
-        <v>46</v>
+        <v>3</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A59" s="1">
-        <v>2324</v>
+        <v>2207</v>
       </c>
       <c r="B59" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A60" s="1">
-        <v>2326</v>
+        <v>2208</v>
       </c>
       <c r="B60" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A61" s="1">
-        <v>2228</v>
+        <v>2213</v>
       </c>
       <c r="B61" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A62" s="1">
-        <v>2328</v>
+        <v>2214</v>
       </c>
       <c r="B62" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A63" s="1">
-        <v>2330</v>
+        <v>2215</v>
       </c>
       <c r="B63" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A64" s="1">
-        <v>2232</v>
+        <v>2216</v>
       </c>
       <c r="B64" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A65" s="1">
-        <v>2332</v>
+        <v>2219</v>
       </c>
       <c r="B65" t="s">
-        <v>53</v>
+        <v>65</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A66" s="1">
-        <v>2334</v>
+        <v>2220</v>
       </c>
       <c r="B66" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A67" s="1">
-        <v>2238</v>
+        <v>2225</v>
       </c>
       <c r="B67" t="s">
-        <v>55</v>
+        <v>68</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A68" s="1">
-        <v>2201</v>
+        <v>2226</v>
       </c>
       <c r="B68" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A69" s="1">
-        <v>2203</v>
+        <v>2228</v>
       </c>
       <c r="B69" t="s">
-        <v>3</v>
+        <v>49</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A70" s="1">
-        <v>2205</v>
+        <v>2229</v>
       </c>
       <c r="B70" t="s">
-        <v>57</v>
+        <v>71</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A71" s="1">
-        <v>2207</v>
+        <v>2231</v>
       </c>
       <c r="B71" t="s">
-        <v>58</v>
+        <v>74</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A72" s="1">
-        <v>2213</v>
+        <v>2232</v>
       </c>
       <c r="B72" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A73" s="1">
-        <v>2111</v>
+        <v>2237</v>
       </c>
       <c r="B73" t="s">
-        <v>60</v>
+        <v>77</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A74" s="1">
-        <v>2113</v>
+        <v>2238</v>
       </c>
       <c r="B74" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A75" s="1">
-        <v>2215</v>
+        <v>2261</v>
       </c>
       <c r="B75" t="s">
-        <v>62</v>
+        <v>89</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A76" s="1">
-        <v>2115</v>
+        <v>2262</v>
       </c>
       <c r="B76" t="s">
-        <v>63</v>
+        <v>88</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A77" s="1">
-        <v>2117</v>
+        <v>2302</v>
       </c>
       <c r="B77" t="s">
-        <v>64</v>
+        <v>3</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A78" s="1">
-        <v>2219</v>
+        <v>2304</v>
       </c>
       <c r="B78" t="s">
-        <v>65</v>
+        <v>3</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A79" s="1">
-        <v>2119</v>
+        <v>2312</v>
       </c>
       <c r="B79" t="s">
-        <v>66</v>
+        <v>38</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A80" s="1">
-        <v>2121</v>
+        <v>2314</v>
       </c>
       <c r="B80" t="s">
-        <v>67</v>
+        <v>39</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A81" s="1">
-        <v>2225</v>
+        <v>2316</v>
       </c>
       <c r="B81" t="s">
-        <v>68</v>
+        <v>41</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A82" s="1">
-        <v>2123</v>
+        <v>2318</v>
       </c>
       <c r="B82" t="s">
-        <v>69</v>
+        <v>42</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A83" s="1">
-        <v>2125</v>
+        <v>2320</v>
       </c>
       <c r="B83" t="s">
-        <v>70</v>
+        <v>44</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A84" s="1">
-        <v>2229</v>
+        <v>2322</v>
       </c>
       <c r="B84" t="s">
-        <v>71</v>
+        <v>45</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A85" s="1">
-        <v>2127</v>
+        <v>2324</v>
       </c>
       <c r="B85" t="s">
-        <v>72</v>
+        <v>47</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A86" s="1">
-        <v>2129</v>
+        <v>2326</v>
       </c>
       <c r="B86" t="s">
-        <v>73</v>
+        <v>48</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A87" s="1">
-        <v>2231</v>
+        <v>2328</v>
       </c>
       <c r="B87" t="s">
-        <v>74</v>
+        <v>50</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A88" s="1">
-        <v>2131</v>
+        <v>2330</v>
       </c>
       <c r="B88" t="s">
-        <v>75</v>
+        <v>51</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A89" s="1">
-        <v>2133</v>
+        <v>2332</v>
       </c>
       <c r="B89" t="s">
-        <v>76</v>
+        <v>53</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A90" s="1">
-        <v>2237</v>
+        <v>2334</v>
       </c>
       <c r="B90" t="s">
-        <v>77</v>
+        <v>54</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A91" s="1">
-        <v>2262</v>
+      <c r="A91" s="1" t="s">
+        <v>30</v>
       </c>
       <c r="B91" t="s">
-        <v>88</v>
+        <v>31</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A92" s="1">
-        <v>2261</v>
+      <c r="A92" s="1" t="s">
+        <v>33</v>
       </c>
       <c r="B92" t="s">
-        <v>89</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C92">
+    <sortCondition ref="A1:A92"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="2a76394f-0ef1-4647-b1d7-82262634529b" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1605,17 +1607,26 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="2a76394f-0ef1-4647-b1d7-82262634529b" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{86328747-DD58-421D-B445-C23F9D2B9A21}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{64810535-1C87-43A1-ADF2-EBA95ECCC978}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="2a76394f-0ef1-4647-b1d7-82262634529b"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1639,17 +1650,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{64810535-1C87-43A1-ADF2-EBA95ECCC978}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{86328747-DD58-421D-B445-C23F9D2B9A21}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="2a76394f-0ef1-4647-b1d7-82262634529b"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>